<commit_message>
added jordans pitching scraping stuff
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="128">
   <si>
     <t>OBP</t>
   </si>
@@ -170,6 +170,234 @@
   </si>
   <si>
     <t>.625</t>
+  </si>
+  <si>
+    <t>.308</t>
+  </si>
+  <si>
+    <t>Sabathia</t>
+  </si>
+  <si>
+    <t>.154</t>
+  </si>
+  <si>
+    <t>.091</t>
+  </si>
+  <si>
+    <t>.077</t>
+  </si>
+  <si>
+    <t>.417</t>
+  </si>
+  <si>
+    <t>.917</t>
+  </si>
+  <si>
+    <t>.182</t>
+  </si>
+  <si>
+    <t>Carpenter</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Steven Tolleson</t>
+  </si>
+  <si>
+    <t>.200</t>
+  </si>
+  <si>
+    <t>Rogers</t>
+  </si>
+  <si>
+    <t>.455</t>
+  </si>
+  <si>
+    <t>NYA</t>
+  </si>
+  <si>
+    <t>NewYorkYankees</t>
+  </si>
+  <si>
+    <t>BAL</t>
+  </si>
+  <si>
+    <t>Jacoby Ellsbury</t>
+  </si>
+  <si>
+    <t>Hutchison</t>
+  </si>
+  <si>
+    <t>Brett Gardner</t>
+  </si>
+  <si>
+    <t>Carlos Beltran</t>
+  </si>
+  <si>
+    <t>Mark Teixeira</t>
+  </si>
+  <si>
+    <t>Brian McCann</t>
+  </si>
+  <si>
+    <t>Chase Headley</t>
+  </si>
+  <si>
+    <t>Alex Rodriguez</t>
+  </si>
+  <si>
+    <t>Stephen Drew</t>
+  </si>
+  <si>
+    <t>Didi Gregorius</t>
+  </si>
+  <si>
+    <t>Dickey</t>
+  </si>
+  <si>
+    <t>.286</t>
+  </si>
+  <si>
+    <t>.167</t>
+  </si>
+  <si>
+    <t>Chris Young</t>
+  </si>
+  <si>
+    <t>Loup</t>
+  </si>
+  <si>
+    <t>.385</t>
+  </si>
+  <si>
+    <t>.273</t>
+  </si>
+  <si>
+    <t>Norris</t>
+  </si>
+  <si>
+    <t>.364</t>
+  </si>
+  <si>
+    <t>.556</t>
+  </si>
+  <si>
+    <t>.600</t>
+  </si>
+  <si>
+    <t>John Ryan Murphy</t>
+  </si>
+  <si>
+    <t>Gregorio Petit</t>
+  </si>
+  <si>
+    <t>Osuna</t>
+  </si>
+  <si>
+    <t>1.250</t>
+  </si>
+  <si>
+    <t>BOS</t>
+  </si>
+  <si>
+    <t>BostonRedSox</t>
+  </si>
+  <si>
+    <t>CLE</t>
+  </si>
+  <si>
+    <t>Mookie Betts</t>
+  </si>
+  <si>
+    <t>Hamels</t>
+  </si>
+  <si>
+    <t>1.800</t>
+  </si>
+  <si>
+    <t>Dustin Pedroia</t>
+  </si>
+  <si>
+    <t>David Ortiz</t>
+  </si>
+  <si>
+    <t>Mike Napoli</t>
+  </si>
+  <si>
+    <t>Diekman</t>
+  </si>
+  <si>
+    <t>Hanley Ramirez</t>
+  </si>
+  <si>
+    <t>Pablo Sandoval</t>
+  </si>
+  <si>
+    <t>Shane Victorino</t>
+  </si>
+  <si>
+    <t>Xander Bogaerts</t>
+  </si>
+  <si>
+    <t>Ryan Hanigan</t>
+  </si>
+  <si>
+    <t>Clay Buchholz</t>
+  </si>
+  <si>
+    <t>Allen Craig</t>
+  </si>
+  <si>
+    <t>Harang</t>
+  </si>
+  <si>
+    <t>1.286</t>
+  </si>
+  <si>
+    <t>Daniel Nava</t>
+  </si>
+  <si>
+    <t>.429</t>
+  </si>
+  <si>
+    <t>Rick Porcello</t>
+  </si>
+  <si>
+    <t>Giles</t>
+  </si>
+  <si>
+    <t>.462</t>
+  </si>
+  <si>
+    <t>Buchanan</t>
+  </si>
+  <si>
+    <t>.357</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>.769</t>
+  </si>
+  <si>
+    <t>.545</t>
+  </si>
+  <si>
+    <t>Justin Masterson</t>
+  </si>
+  <si>
+    <t>Fratus</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Craig Breslow</t>
+  </si>
+  <si>
+    <t>Brock Holt</t>
   </si>
 </sst>
 </file>
@@ -523,7 +751,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1493,6 +1721,3552 @@
         <v>0</v>
       </c>
     </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" t="s"/>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="s">
+        <v>53</v>
+      </c>
+      <c r="N21" t="n">
+        <v>2</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" t="s"/>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="s">
+        <v>53</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" t="s"/>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="s">
+        <v>53</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" t="s"/>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="s">
+        <v>53</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s"/>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="s">
+        <v>53</v>
+      </c>
+      <c r="N25" t="n">
+        <v>2</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" t="s"/>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" t="s">
+        <v>49</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="s">
+        <v>53</v>
+      </c>
+      <c r="N26" t="n">
+        <v>2</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" t="s"/>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>21</v>
+      </c>
+      <c r="K27" t="s">
+        <v>47</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="s">
+        <v>60</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" t="s"/>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="s">
+        <v>53</v>
+      </c>
+      <c r="N28" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" t="s"/>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" t="s">
+        <v>62</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="s">
+        <v>53</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" t="s"/>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" t="s">
+        <v>32</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="s">
+        <v>64</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" t="s"/>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" t="s">
+        <v>37</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="s">
+        <v>53</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" t="s"/>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>68</v>
+      </c>
+      <c r="K32" t="s">
+        <v>69</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="s">
+        <v>70</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" t="s"/>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>68</v>
+      </c>
+      <c r="K33" t="s">
+        <v>71</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="s">
+        <v>70</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" t="s"/>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" t="s">
+        <v>72</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="s">
+        <v>70</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" t="s"/>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="s">
+        <v>68</v>
+      </c>
+      <c r="K35" t="s">
+        <v>73</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" t="s">
+        <v>70</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" t="s"/>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" t="s">
+        <v>74</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" t="s">
+        <v>70</v>
+      </c>
+      <c r="N36" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" t="s"/>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="s">
+        <v>68</v>
+      </c>
+      <c r="K37" t="s">
+        <v>75</v>
+      </c>
+      <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="s">
+        <v>70</v>
+      </c>
+      <c r="N37" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" t="s">
+        <v>67</v>
+      </c>
+      <c r="F38" t="s"/>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="s">
+        <v>68</v>
+      </c>
+      <c r="K38" t="s">
+        <v>76</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="s">
+        <v>70</v>
+      </c>
+      <c r="N38" t="n">
+        <v>1</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" t="s"/>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>68</v>
+      </c>
+      <c r="K39" t="s">
+        <v>77</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="s">
+        <v>70</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" t="s"/>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>68</v>
+      </c>
+      <c r="K40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" t="s">
+        <v>70</v>
+      </c>
+      <c r="N40" t="n">
+        <v>0</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" t="s"/>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="s">
+        <v>68</v>
+      </c>
+      <c r="K41" t="s">
+        <v>69</v>
+      </c>
+      <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="s">
+        <v>79</v>
+      </c>
+      <c r="N41" t="n">
+        <v>2</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0</v>
+      </c>
+      <c r="P41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" t="s">
+        <v>67</v>
+      </c>
+      <c r="F42" t="s"/>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="s">
+        <v>68</v>
+      </c>
+      <c r="K42" t="s">
+        <v>71</v>
+      </c>
+      <c r="L42" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="s">
+        <v>79</v>
+      </c>
+      <c r="N42" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43" t="s"/>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="s">
+        <v>68</v>
+      </c>
+      <c r="K43" t="s">
+        <v>72</v>
+      </c>
+      <c r="L43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" t="s">
+        <v>79</v>
+      </c>
+      <c r="N43" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" t="s"/>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="s">
+        <v>68</v>
+      </c>
+      <c r="K44" t="s">
+        <v>73</v>
+      </c>
+      <c r="L44" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" t="s">
+        <v>79</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" t="s">
+        <v>67</v>
+      </c>
+      <c r="F45" t="s"/>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="s">
+        <v>68</v>
+      </c>
+      <c r="K45" t="s">
+        <v>74</v>
+      </c>
+      <c r="L45" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" t="s">
+        <v>79</v>
+      </c>
+      <c r="N45" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" t="s">
+        <v>67</v>
+      </c>
+      <c r="F46" t="s"/>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="s">
+        <v>68</v>
+      </c>
+      <c r="K46" t="s">
+        <v>75</v>
+      </c>
+      <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="s">
+        <v>79</v>
+      </c>
+      <c r="N46" t="n">
+        <v>2</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47" t="s">
+        <v>67</v>
+      </c>
+      <c r="F47" t="s"/>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="s">
+        <v>68</v>
+      </c>
+      <c r="K47" t="s">
+        <v>76</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
+      <c r="M47" t="s">
+        <v>79</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48" t="s">
+        <v>67</v>
+      </c>
+      <c r="F48" t="s"/>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="s">
+        <v>68</v>
+      </c>
+      <c r="K48" t="s">
+        <v>77</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0</v>
+      </c>
+      <c r="M48" t="s">
+        <v>79</v>
+      </c>
+      <c r="N48" t="n">
+        <v>1</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0</v>
+      </c>
+      <c r="P48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" t="s">
+        <v>66</v>
+      </c>
+      <c r="E49" t="s">
+        <v>67</v>
+      </c>
+      <c r="F49" t="s"/>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="s">
+        <v>68</v>
+      </c>
+      <c r="K49" t="s">
+        <v>78</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" t="s">
+        <v>79</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
+        <v>36</v>
+      </c>
+      <c r="D50" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" t="s">
+        <v>67</v>
+      </c>
+      <c r="F50" t="s"/>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="s">
+        <v>68</v>
+      </c>
+      <c r="K50" t="s">
+        <v>82</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0</v>
+      </c>
+      <c r="M50" t="s">
+        <v>83</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0</v>
+      </c>
+      <c r="O50" t="n">
+        <v>0</v>
+      </c>
+      <c r="P50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" t="s">
+        <v>67</v>
+      </c>
+      <c r="F51" t="s"/>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="s">
+        <v>68</v>
+      </c>
+      <c r="K51" t="s">
+        <v>69</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" t="s">
+        <v>86</v>
+      </c>
+      <c r="N51" t="n">
+        <v>1</v>
+      </c>
+      <c r="O51" t="n">
+        <v>0</v>
+      </c>
+      <c r="P51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" t="s">
+        <v>66</v>
+      </c>
+      <c r="E52" t="s">
+        <v>67</v>
+      </c>
+      <c r="F52" t="s"/>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="n">
+        <v>1</v>
+      </c>
+      <c r="J52" t="s">
+        <v>68</v>
+      </c>
+      <c r="K52" t="s">
+        <v>76</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" t="s">
+        <v>86</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0</v>
+      </c>
+      <c r="P52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" t="s">
+        <v>66</v>
+      </c>
+      <c r="E53" t="s">
+        <v>67</v>
+      </c>
+      <c r="F53" t="s"/>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>1</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>68</v>
+      </c>
+      <c r="K53" t="s">
+        <v>72</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" t="s">
+        <v>86</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0</v>
+      </c>
+      <c r="P53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="A54" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" t="s">
+        <v>89</v>
+      </c>
+      <c r="D54" t="s">
+        <v>66</v>
+      </c>
+      <c r="E54" t="s">
+        <v>67</v>
+      </c>
+      <c r="F54" t="s"/>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="n">
+        <v>1</v>
+      </c>
+      <c r="J54" t="s">
+        <v>68</v>
+      </c>
+      <c r="K54" t="s">
+        <v>73</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" t="s">
+        <v>86</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0</v>
+      </c>
+      <c r="O54" t="n">
+        <v>0</v>
+      </c>
+      <c r="P54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" t="s">
+        <v>66</v>
+      </c>
+      <c r="E55" t="s">
+        <v>67</v>
+      </c>
+      <c r="F55" t="s"/>
+      <c r="G55" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="s">
+        <v>68</v>
+      </c>
+      <c r="K55" t="s">
+        <v>75</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0</v>
+      </c>
+      <c r="M55" t="s">
+        <v>86</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0</v>
+      </c>
+      <c r="O55" t="n">
+        <v>0</v>
+      </c>
+      <c r="P55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" t="s">
+        <v>46</v>
+      </c>
+      <c r="D56" t="s">
+        <v>66</v>
+      </c>
+      <c r="E56" t="s">
+        <v>67</v>
+      </c>
+      <c r="F56" t="s"/>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="s">
+        <v>68</v>
+      </c>
+      <c r="K56" t="s">
+        <v>82</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0</v>
+      </c>
+      <c r="M56" t="s">
+        <v>86</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0</v>
+      </c>
+      <c r="P56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="A57" t="s">
+        <v>33</v>
+      </c>
+      <c r="B57" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" t="s">
+        <v>66</v>
+      </c>
+      <c r="E57" t="s">
+        <v>67</v>
+      </c>
+      <c r="F57" t="s"/>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" t="n">
+        <v>2</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="s">
+        <v>68</v>
+      </c>
+      <c r="K57" t="s">
+        <v>90</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0</v>
+      </c>
+      <c r="M57" t="s">
+        <v>86</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0</v>
+      </c>
+      <c r="O57" t="n">
+        <v>0</v>
+      </c>
+      <c r="P57" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" t="s">
+        <v>66</v>
+      </c>
+      <c r="E58" t="s">
+        <v>67</v>
+      </c>
+      <c r="F58" t="s"/>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="s">
+        <v>68</v>
+      </c>
+      <c r="K58" t="s">
+        <v>91</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0</v>
+      </c>
+      <c r="M58" t="s">
+        <v>86</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59" t="s">
+        <v>66</v>
+      </c>
+      <c r="E59" t="s">
+        <v>67</v>
+      </c>
+      <c r="F59" t="s"/>
+      <c r="G59" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="s">
+        <v>68</v>
+      </c>
+      <c r="K59" t="s">
+        <v>77</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0</v>
+      </c>
+      <c r="M59" t="s">
+        <v>92</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0</v>
+      </c>
+      <c r="O59" t="n">
+        <v>0</v>
+      </c>
+      <c r="P59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
+      <c r="A60" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" t="s">
+        <v>66</v>
+      </c>
+      <c r="E60" t="s">
+        <v>67</v>
+      </c>
+      <c r="F60" t="s"/>
+      <c r="G60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="s">
+        <v>68</v>
+      </c>
+      <c r="K60" t="s">
+        <v>78</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" t="s">
+        <v>86</v>
+      </c>
+      <c r="N60" t="n">
+        <v>1</v>
+      </c>
+      <c r="O60" t="n">
+        <v>0</v>
+      </c>
+      <c r="P60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
+      <c r="A61" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61" t="s">
+        <v>94</v>
+      </c>
+      <c r="E61" t="s">
+        <v>95</v>
+      </c>
+      <c r="F61" t="s"/>
+      <c r="G61" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" t="s">
+        <v>96</v>
+      </c>
+      <c r="K61" t="s">
+        <v>97</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" t="s">
+        <v>98</v>
+      </c>
+      <c r="N61" t="n">
+        <v>1</v>
+      </c>
+      <c r="O61" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
+      <c r="A62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" t="s">
+        <v>99</v>
+      </c>
+      <c r="D62" t="s">
+        <v>94</v>
+      </c>
+      <c r="E62" t="s">
+        <v>95</v>
+      </c>
+      <c r="F62" t="s"/>
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="n">
+        <v>2</v>
+      </c>
+      <c r="J62" t="s">
+        <v>96</v>
+      </c>
+      <c r="K62" t="s">
+        <v>100</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0</v>
+      </c>
+      <c r="M62" t="s">
+        <v>98</v>
+      </c>
+      <c r="N62" t="n">
+        <v>1</v>
+      </c>
+      <c r="O62" t="n">
+        <v>0</v>
+      </c>
+      <c r="P62" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
+      <c r="A63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" t="s">
+        <v>94</v>
+      </c>
+      <c r="E63" t="s">
+        <v>95</v>
+      </c>
+      <c r="F63" t="s"/>
+      <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+      <c r="J63" t="s">
+        <v>96</v>
+      </c>
+      <c r="K63" t="s">
+        <v>101</v>
+      </c>
+      <c r="L63" t="n">
+        <v>0</v>
+      </c>
+      <c r="M63" t="s">
+        <v>98</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0</v>
+      </c>
+      <c r="O63" t="n">
+        <v>0</v>
+      </c>
+      <c r="P63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
+      <c r="A64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" t="s"/>
+      <c r="D64" t="s">
+        <v>94</v>
+      </c>
+      <c r="E64" t="s">
+        <v>95</v>
+      </c>
+      <c r="F64" t="s"/>
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="s">
+        <v>96</v>
+      </c>
+      <c r="K64" t="s">
+        <v>102</v>
+      </c>
+      <c r="L64" t="n">
+        <v>0</v>
+      </c>
+      <c r="M64" t="s">
+        <v>103</v>
+      </c>
+      <c r="N64" t="n">
+        <v>0</v>
+      </c>
+      <c r="O64" t="n">
+        <v>0</v>
+      </c>
+      <c r="P64" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
+      <c r="A65" t="s">
+        <v>89</v>
+      </c>
+      <c r="B65" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" t="s">
+        <v>36</v>
+      </c>
+      <c r="D65" t="s">
+        <v>94</v>
+      </c>
+      <c r="E65" t="s">
+        <v>95</v>
+      </c>
+      <c r="F65" t="s"/>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
+        <v>1</v>
+      </c>
+      <c r="I65" t="n">
+        <v>2</v>
+      </c>
+      <c r="J65" t="s">
+        <v>96</v>
+      </c>
+      <c r="K65" t="s">
+        <v>104</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0</v>
+      </c>
+      <c r="M65" t="s">
+        <v>98</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0</v>
+      </c>
+      <c r="O65" t="n">
+        <v>0</v>
+      </c>
+      <c r="P65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
+      <c r="A66" t="s">
+        <v>18</v>
+      </c>
+      <c r="B66" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" t="s">
+        <v>18</v>
+      </c>
+      <c r="D66" t="s">
+        <v>94</v>
+      </c>
+      <c r="E66" t="s">
+        <v>95</v>
+      </c>
+      <c r="F66" t="s"/>
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" t="s">
+        <v>96</v>
+      </c>
+      <c r="K66" t="s">
+        <v>105</v>
+      </c>
+      <c r="L66" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" t="s">
+        <v>98</v>
+      </c>
+      <c r="N66" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
+      <c r="A67" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" t="s">
+        <v>94</v>
+      </c>
+      <c r="E67" t="s">
+        <v>95</v>
+      </c>
+      <c r="F67" t="s"/>
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" t="s">
+        <v>96</v>
+      </c>
+      <c r="K67" t="s">
+        <v>106</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0</v>
+      </c>
+      <c r="M67" t="s">
+        <v>98</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0</v>
+      </c>
+      <c r="O67" t="n">
+        <v>0</v>
+      </c>
+      <c r="P67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16">
+      <c r="A68" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" t="s">
+        <v>94</v>
+      </c>
+      <c r="E68" t="s">
+        <v>95</v>
+      </c>
+      <c r="F68" t="s"/>
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" t="s">
+        <v>96</v>
+      </c>
+      <c r="K68" t="s">
+        <v>107</v>
+      </c>
+      <c r="L68" t="n">
+        <v>0</v>
+      </c>
+      <c r="M68" t="s">
+        <v>98</v>
+      </c>
+      <c r="N68" t="n">
+        <v>0</v>
+      </c>
+      <c r="O68" t="n">
+        <v>0</v>
+      </c>
+      <c r="P68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
+      <c r="A69" t="s">
+        <v>33</v>
+      </c>
+      <c r="B69" t="s">
+        <v>27</v>
+      </c>
+      <c r="C69" t="s">
+        <v>44</v>
+      </c>
+      <c r="D69" t="s">
+        <v>94</v>
+      </c>
+      <c r="E69" t="s">
+        <v>95</v>
+      </c>
+      <c r="F69" t="s"/>
+      <c r="G69" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="s">
+        <v>96</v>
+      </c>
+      <c r="K69" t="s">
+        <v>108</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0</v>
+      </c>
+      <c r="M69" t="s">
+        <v>98</v>
+      </c>
+      <c r="N69" t="n">
+        <v>1</v>
+      </c>
+      <c r="O69" t="n">
+        <v>0</v>
+      </c>
+      <c r="P69" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
+      <c r="A70" t="s">
+        <v>18</v>
+      </c>
+      <c r="B70" t="s">
+        <v>45</v>
+      </c>
+      <c r="C70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" t="s">
+        <v>94</v>
+      </c>
+      <c r="E70" t="s">
+        <v>95</v>
+      </c>
+      <c r="F70" t="s"/>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="s">
+        <v>96</v>
+      </c>
+      <c r="K70" t="s">
+        <v>109</v>
+      </c>
+      <c r="L70" t="n">
+        <v>0</v>
+      </c>
+      <c r="M70" t="s">
+        <v>98</v>
+      </c>
+      <c r="N70" t="n">
+        <v>0</v>
+      </c>
+      <c r="O70" t="n">
+        <v>0</v>
+      </c>
+      <c r="P70" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16">
+      <c r="A71" t="s">
+        <v>28</v>
+      </c>
+      <c r="B71" t="s">
+        <v>48</v>
+      </c>
+      <c r="C71" t="s">
+        <v>28</v>
+      </c>
+      <c r="D71" t="s">
+        <v>94</v>
+      </c>
+      <c r="E71" t="s">
+        <v>95</v>
+      </c>
+      <c r="F71" t="s"/>
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" t="s">
+        <v>96</v>
+      </c>
+      <c r="K71" t="s">
+        <v>110</v>
+      </c>
+      <c r="L71" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" t="s">
+        <v>103</v>
+      </c>
+      <c r="N71" t="n">
+        <v>1</v>
+      </c>
+      <c r="O71" t="n">
+        <v>0</v>
+      </c>
+      <c r="P71" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
+      <c r="A72" t="s">
+        <v>44</v>
+      </c>
+      <c r="B72" t="s">
+        <v>27</v>
+      </c>
+      <c r="C72" t="s">
+        <v>51</v>
+      </c>
+      <c r="D72" t="s">
+        <v>94</v>
+      </c>
+      <c r="E72" t="s">
+        <v>95</v>
+      </c>
+      <c r="F72" t="s"/>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" t="s">
+        <v>96</v>
+      </c>
+      <c r="K72" t="s">
+        <v>97</v>
+      </c>
+      <c r="L72" t="n">
+        <v>0</v>
+      </c>
+      <c r="M72" t="s">
+        <v>111</v>
+      </c>
+      <c r="N72" t="n">
+        <v>0</v>
+      </c>
+      <c r="O72" t="n">
+        <v>0</v>
+      </c>
+      <c r="P72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
+      <c r="A73" t="s">
+        <v>88</v>
+      </c>
+      <c r="B73" t="s">
+        <v>27</v>
+      </c>
+      <c r="C73" t="s">
+        <v>112</v>
+      </c>
+      <c r="D73" t="s">
+        <v>94</v>
+      </c>
+      <c r="E73" t="s">
+        <v>95</v>
+      </c>
+      <c r="F73" t="s"/>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" t="s">
+        <v>96</v>
+      </c>
+      <c r="K73" t="s">
+        <v>100</v>
+      </c>
+      <c r="L73" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" t="s">
+        <v>111</v>
+      </c>
+      <c r="N73" t="n">
+        <v>0</v>
+      </c>
+      <c r="O73" t="n">
+        <v>0</v>
+      </c>
+      <c r="P73" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
+      <c r="A74" t="s">
+        <v>44</v>
+      </c>
+      <c r="B74" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" t="s">
+        <v>94</v>
+      </c>
+      <c r="E74" t="s">
+        <v>95</v>
+      </c>
+      <c r="F74" t="s"/>
+      <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" t="s">
+        <v>96</v>
+      </c>
+      <c r="K74" t="s">
+        <v>105</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" t="s">
+        <v>111</v>
+      </c>
+      <c r="N74" t="n">
+        <v>2</v>
+      </c>
+      <c r="O74" t="n">
+        <v>0</v>
+      </c>
+      <c r="P74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16">
+      <c r="A75" t="s">
+        <v>44</v>
+      </c>
+      <c r="B75" t="s">
+        <v>27</v>
+      </c>
+      <c r="C75" t="s">
+        <v>28</v>
+      </c>
+      <c r="D75" t="s">
+        <v>94</v>
+      </c>
+      <c r="E75" t="s">
+        <v>95</v>
+      </c>
+      <c r="F75" t="s"/>
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" t="s">
+        <v>96</v>
+      </c>
+      <c r="K75" t="s">
+        <v>104</v>
+      </c>
+      <c r="L75" t="n">
+        <v>0</v>
+      </c>
+      <c r="M75" t="s">
+        <v>111</v>
+      </c>
+      <c r="N75" t="n">
+        <v>0</v>
+      </c>
+      <c r="O75" t="n">
+        <v>0</v>
+      </c>
+      <c r="P75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
+      <c r="A76" t="s">
+        <v>63</v>
+      </c>
+      <c r="B76" t="s">
+        <v>27</v>
+      </c>
+      <c r="C76" t="s">
+        <v>18</v>
+      </c>
+      <c r="D76" t="s">
+        <v>94</v>
+      </c>
+      <c r="E76" t="s">
+        <v>95</v>
+      </c>
+      <c r="F76" t="s"/>
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" t="n">
+        <v>1</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" t="s">
+        <v>96</v>
+      </c>
+      <c r="K76" t="s">
+        <v>102</v>
+      </c>
+      <c r="L76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M76" t="s">
+        <v>111</v>
+      </c>
+      <c r="N76" t="n">
+        <v>0</v>
+      </c>
+      <c r="O76" t="n">
+        <v>0</v>
+      </c>
+      <c r="P76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
+      <c r="A77" t="s">
+        <v>18</v>
+      </c>
+      <c r="B77" t="s">
+        <v>27</v>
+      </c>
+      <c r="C77" t="s">
+        <v>18</v>
+      </c>
+      <c r="D77" t="s">
+        <v>94</v>
+      </c>
+      <c r="E77" t="s">
+        <v>95</v>
+      </c>
+      <c r="F77" t="s"/>
+      <c r="G77" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" t="s">
+        <v>96</v>
+      </c>
+      <c r="K77" t="s">
+        <v>113</v>
+      </c>
+      <c r="L77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M77" t="s">
+        <v>111</v>
+      </c>
+      <c r="N77" t="n">
+        <v>0</v>
+      </c>
+      <c r="O77" t="n">
+        <v>0</v>
+      </c>
+      <c r="P77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16">
+      <c r="A78" t="s">
+        <v>114</v>
+      </c>
+      <c r="B78" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78" t="s">
+        <v>63</v>
+      </c>
+      <c r="D78" t="s">
+        <v>94</v>
+      </c>
+      <c r="E78" t="s">
+        <v>95</v>
+      </c>
+      <c r="F78" t="s"/>
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" t="s">
+        <v>96</v>
+      </c>
+      <c r="K78" t="s">
+        <v>108</v>
+      </c>
+      <c r="L78" t="n">
+        <v>0</v>
+      </c>
+      <c r="M78" t="s">
+        <v>111</v>
+      </c>
+      <c r="N78" t="n">
+        <v>0</v>
+      </c>
+      <c r="O78" t="n">
+        <v>0</v>
+      </c>
+      <c r="P78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16">
+      <c r="A79" t="s">
+        <v>16</v>
+      </c>
+      <c r="B79" t="s">
+        <v>27</v>
+      </c>
+      <c r="C79" t="s">
+        <v>41</v>
+      </c>
+      <c r="D79" t="s">
+        <v>94</v>
+      </c>
+      <c r="E79" t="s">
+        <v>95</v>
+      </c>
+      <c r="F79" t="s"/>
+      <c r="G79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" t="s">
+        <v>96</v>
+      </c>
+      <c r="K79" t="s">
+        <v>107</v>
+      </c>
+      <c r="L79" t="n">
+        <v>0</v>
+      </c>
+      <c r="M79" t="s">
+        <v>111</v>
+      </c>
+      <c r="N79" t="n">
+        <v>1</v>
+      </c>
+      <c r="O79" t="n">
+        <v>0</v>
+      </c>
+      <c r="P79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16">
+      <c r="A80" t="s">
+        <v>18</v>
+      </c>
+      <c r="B80" t="s">
+        <v>61</v>
+      </c>
+      <c r="C80" t="s">
+        <v>18</v>
+      </c>
+      <c r="D80" t="s">
+        <v>94</v>
+      </c>
+      <c r="E80" t="s">
+        <v>95</v>
+      </c>
+      <c r="F80" t="s"/>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" t="s">
+        <v>96</v>
+      </c>
+      <c r="K80" t="s">
+        <v>115</v>
+      </c>
+      <c r="L80" t="n">
+        <v>0</v>
+      </c>
+      <c r="M80" t="s">
+        <v>111</v>
+      </c>
+      <c r="N80" t="n">
+        <v>0</v>
+      </c>
+      <c r="O80" t="n">
+        <v>0</v>
+      </c>
+      <c r="P80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16">
+      <c r="A81" t="s">
+        <v>18</v>
+      </c>
+      <c r="B81" t="s">
+        <v>48</v>
+      </c>
+      <c r="C81" t="s">
+        <v>18</v>
+      </c>
+      <c r="D81" t="s">
+        <v>94</v>
+      </c>
+      <c r="E81" t="s">
+        <v>95</v>
+      </c>
+      <c r="F81" t="s"/>
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" t="s">
+        <v>96</v>
+      </c>
+      <c r="K81" t="s">
+        <v>101</v>
+      </c>
+      <c r="L81" t="n">
+        <v>0</v>
+      </c>
+      <c r="M81" t="s">
+        <v>116</v>
+      </c>
+      <c r="N81" t="n">
+        <v>0</v>
+      </c>
+      <c r="O81" t="n">
+        <v>0</v>
+      </c>
+      <c r="P81" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16">
+      <c r="A82" t="s">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>17</v>
+      </c>
+      <c r="C82" t="s">
+        <v>117</v>
+      </c>
+      <c r="D82" t="s">
+        <v>94</v>
+      </c>
+      <c r="E82" t="s">
+        <v>95</v>
+      </c>
+      <c r="F82" t="s"/>
+      <c r="G82" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
+      <c r="I82" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" t="s">
+        <v>96</v>
+      </c>
+      <c r="K82" t="s">
+        <v>97</v>
+      </c>
+      <c r="L82" t="n">
+        <v>0</v>
+      </c>
+      <c r="M82" t="s">
+        <v>118</v>
+      </c>
+      <c r="N82" t="n">
+        <v>1</v>
+      </c>
+      <c r="O82" t="n">
+        <v>0</v>
+      </c>
+      <c r="P82" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16">
+      <c r="A83" t="s">
+        <v>119</v>
+      </c>
+      <c r="B83" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83" t="s">
+        <v>35</v>
+      </c>
+      <c r="D83" t="s">
+        <v>94</v>
+      </c>
+      <c r="E83" t="s">
+        <v>95</v>
+      </c>
+      <c r="F83" t="s"/>
+      <c r="G83" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0</v>
+      </c>
+      <c r="I83" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" t="s">
+        <v>96</v>
+      </c>
+      <c r="K83" t="s">
+        <v>100</v>
+      </c>
+      <c r="L83" t="n">
+        <v>0</v>
+      </c>
+      <c r="M83" t="s">
+        <v>118</v>
+      </c>
+      <c r="N83" t="n">
+        <v>0</v>
+      </c>
+      <c r="O83" t="n">
+        <v>0</v>
+      </c>
+      <c r="P83" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16">
+      <c r="A84" t="s">
+        <v>44</v>
+      </c>
+      <c r="B84" t="s">
+        <v>27</v>
+      </c>
+      <c r="C84" t="s">
+        <v>41</v>
+      </c>
+      <c r="D84" t="s">
+        <v>94</v>
+      </c>
+      <c r="E84" t="s">
+        <v>95</v>
+      </c>
+      <c r="F84" t="s"/>
+      <c r="G84" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" t="s">
+        <v>96</v>
+      </c>
+      <c r="K84" t="s">
+        <v>101</v>
+      </c>
+      <c r="L84" t="n">
+        <v>0</v>
+      </c>
+      <c r="M84" t="s">
+        <v>118</v>
+      </c>
+      <c r="N84" t="n">
+        <v>1</v>
+      </c>
+      <c r="O84" t="n">
+        <v>0</v>
+      </c>
+      <c r="P84" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16">
+      <c r="A85" t="s">
+        <v>81</v>
+      </c>
+      <c r="B85" t="s">
+        <v>48</v>
+      </c>
+      <c r="C85" t="s">
+        <v>18</v>
+      </c>
+      <c r="D85" t="s">
+        <v>94</v>
+      </c>
+      <c r="E85" t="s">
+        <v>95</v>
+      </c>
+      <c r="F85" t="s"/>
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" t="s">
+        <v>96</v>
+      </c>
+      <c r="K85" t="s">
+        <v>102</v>
+      </c>
+      <c r="L85" t="n">
+        <v>0</v>
+      </c>
+      <c r="M85" t="s">
+        <v>120</v>
+      </c>
+      <c r="N85" t="n">
+        <v>0</v>
+      </c>
+      <c r="O85" t="n">
+        <v>0</v>
+      </c>
+      <c r="P85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16">
+      <c r="A86" t="s">
+        <v>119</v>
+      </c>
+      <c r="B86" t="s">
+        <v>17</v>
+      </c>
+      <c r="C86" t="s">
+        <v>121</v>
+      </c>
+      <c r="D86" t="s">
+        <v>94</v>
+      </c>
+      <c r="E86" t="s">
+        <v>95</v>
+      </c>
+      <c r="F86" t="s"/>
+      <c r="G86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" t="s">
+        <v>96</v>
+      </c>
+      <c r="K86" t="s">
+        <v>104</v>
+      </c>
+      <c r="L86" t="n">
+        <v>0</v>
+      </c>
+      <c r="M86" t="s">
+        <v>118</v>
+      </c>
+      <c r="N86" t="n">
+        <v>2</v>
+      </c>
+      <c r="O86" t="n">
+        <v>0</v>
+      </c>
+      <c r="P86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16">
+      <c r="A87" t="s">
+        <v>80</v>
+      </c>
+      <c r="B87" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87" t="s">
+        <v>81</v>
+      </c>
+      <c r="D87" t="s">
+        <v>94</v>
+      </c>
+      <c r="E87" t="s">
+        <v>95</v>
+      </c>
+      <c r="F87" t="s"/>
+      <c r="G87" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" t="s">
+        <v>96</v>
+      </c>
+      <c r="K87" t="s">
+        <v>105</v>
+      </c>
+      <c r="L87" t="n">
+        <v>0</v>
+      </c>
+      <c r="M87" t="s">
+        <v>118</v>
+      </c>
+      <c r="N87" t="n">
+        <v>0</v>
+      </c>
+      <c r="O87" t="n">
+        <v>0</v>
+      </c>
+      <c r="P87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16">
+      <c r="A88" t="s">
+        <v>24</v>
+      </c>
+      <c r="B88" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88" t="s">
+        <v>94</v>
+      </c>
+      <c r="E88" t="s">
+        <v>95</v>
+      </c>
+      <c r="F88" t="s"/>
+      <c r="G88" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
+      <c r="J88" t="s">
+        <v>96</v>
+      </c>
+      <c r="K88" t="s">
+        <v>106</v>
+      </c>
+      <c r="L88" t="n">
+        <v>0</v>
+      </c>
+      <c r="M88" t="s">
+        <v>118</v>
+      </c>
+      <c r="N88" t="n">
+        <v>2</v>
+      </c>
+      <c r="O88" t="n">
+        <v>0</v>
+      </c>
+      <c r="P88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16">
+      <c r="A89" t="s">
+        <v>57</v>
+      </c>
+      <c r="B89" t="s">
+        <v>17</v>
+      </c>
+      <c r="C89" t="s">
+        <v>39</v>
+      </c>
+      <c r="D89" t="s">
+        <v>94</v>
+      </c>
+      <c r="E89" t="s">
+        <v>95</v>
+      </c>
+      <c r="F89" t="s"/>
+      <c r="G89" t="n">
+        <v>0</v>
+      </c>
+      <c r="H89" t="n">
+        <v>1</v>
+      </c>
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
+      <c r="J89" t="s">
+        <v>96</v>
+      </c>
+      <c r="K89" t="s">
+        <v>108</v>
+      </c>
+      <c r="L89" t="n">
+        <v>0</v>
+      </c>
+      <c r="M89" t="s">
+        <v>118</v>
+      </c>
+      <c r="N89" t="n">
+        <v>0</v>
+      </c>
+      <c r="O89" t="n">
+        <v>0</v>
+      </c>
+      <c r="P89" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16">
+      <c r="A90" t="s">
+        <v>117</v>
+      </c>
+      <c r="B90" t="s">
+        <v>17</v>
+      </c>
+      <c r="C90" t="s">
+        <v>122</v>
+      </c>
+      <c r="D90" t="s">
+        <v>94</v>
+      </c>
+      <c r="E90" t="s">
+        <v>95</v>
+      </c>
+      <c r="F90" t="s"/>
+      <c r="G90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" t="s">
+        <v>96</v>
+      </c>
+      <c r="K90" t="s">
+        <v>107</v>
+      </c>
+      <c r="L90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M90" t="s">
+        <v>118</v>
+      </c>
+      <c r="N90" t="n">
+        <v>2</v>
+      </c>
+      <c r="O90" t="n">
+        <v>1</v>
+      </c>
+      <c r="P90" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16">
+      <c r="A91" t="s">
+        <v>46</v>
+      </c>
+      <c r="B91" t="s">
+        <v>45</v>
+      </c>
+      <c r="C91" t="s">
+        <v>46</v>
+      </c>
+      <c r="D91" t="s">
+        <v>94</v>
+      </c>
+      <c r="E91" t="s">
+        <v>95</v>
+      </c>
+      <c r="F91" t="s"/>
+      <c r="G91" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
+      <c r="J91" t="s">
+        <v>96</v>
+      </c>
+      <c r="K91" t="s">
+        <v>123</v>
+      </c>
+      <c r="L91" t="n">
+        <v>0</v>
+      </c>
+      <c r="M91" t="s">
+        <v>118</v>
+      </c>
+      <c r="N91" t="n">
+        <v>2</v>
+      </c>
+      <c r="O91" t="n">
+        <v>0</v>
+      </c>
+      <c r="P91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16">
+      <c r="A92" t="s">
+        <v>33</v>
+      </c>
+      <c r="B92" t="s">
+        <v>48</v>
+      </c>
+      <c r="C92" t="s">
+        <v>33</v>
+      </c>
+      <c r="D92" t="s">
+        <v>94</v>
+      </c>
+      <c r="E92" t="s">
+        <v>95</v>
+      </c>
+      <c r="F92" t="s"/>
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" t="s">
+        <v>96</v>
+      </c>
+      <c r="K92" t="s">
+        <v>110</v>
+      </c>
+      <c r="L92" t="n">
+        <v>0</v>
+      </c>
+      <c r="M92" t="s">
+        <v>124</v>
+      </c>
+      <c r="N92" t="n">
+        <v>0</v>
+      </c>
+      <c r="O92" t="n">
+        <v>0</v>
+      </c>
+      <c r="P92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16">
+      <c r="A93" t="s"/>
+      <c r="B93" t="s">
+        <v>125</v>
+      </c>
+      <c r="C93" t="s"/>
+      <c r="D93" t="s">
+        <v>94</v>
+      </c>
+      <c r="E93" t="s">
+        <v>95</v>
+      </c>
+      <c r="F93" t="s"/>
+      <c r="G93" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="n">
+        <v>0</v>
+      </c>
+      <c r="J93" t="s">
+        <v>96</v>
+      </c>
+      <c r="K93" t="s">
+        <v>126</v>
+      </c>
+      <c r="L93" t="n">
+        <v>0</v>
+      </c>
+      <c r="M93" t="s">
+        <v>124</v>
+      </c>
+      <c r="N93" t="n">
+        <v>0</v>
+      </c>
+      <c r="O93" t="n">
+        <v>0</v>
+      </c>
+      <c r="P93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16">
+      <c r="A94" t="s">
+        <v>18</v>
+      </c>
+      <c r="B94" t="s">
+        <v>48</v>
+      </c>
+      <c r="C94" t="s">
+        <v>18</v>
+      </c>
+      <c r="D94" t="s">
+        <v>94</v>
+      </c>
+      <c r="E94" t="s">
+        <v>95</v>
+      </c>
+      <c r="F94" t="s"/>
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" t="s">
+        <v>96</v>
+      </c>
+      <c r="K94" t="s">
+        <v>127</v>
+      </c>
+      <c r="L94" t="n">
+        <v>0</v>
+      </c>
+      <c r="M94" t="s">
+        <v>103</v>
+      </c>
+      <c r="N94" t="n">
+        <v>0</v>
+      </c>
+      <c r="O94" t="n">
+        <v>0</v>
+      </c>
+      <c r="P94" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>